<commit_message>
Agregada interaccion basica a traves de controladores
</commit_message>
<xml_diff>
--- a/CrombieConsole/BibliotecaBaseDatos.xlsx
+++ b/CrombieConsole/BibliotecaBaseDatos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\migue\source\repos\Crombie\CrombieConsole\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{312BAEC8-EFD9-48E0-8115-F7AE693F3E56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{109399A2-D635-439E-A853-71DAC24D1E75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <x:bookViews>
-    <x:workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="0" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <x:workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="0" activeTab="0" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </x:bookViews>
   <x:sheets>
     <x:sheet name="Usuarios" sheetId="1" r:id="rId1"/>
@@ -34,102 +34,108 @@
     <x:t>TipoUsuario</x:t>
   </x:si>
   <x:si>
-    <x:t>LibrosPrestados</x:t>
-  </x:si>
-  <x:si>
     <x:t>Juan</x:t>
   </x:si>
   <x:si>
     <x:t>Estudiante</x:t>
   </x:si>
   <x:si>
+    <x:t>Dr. Ana</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Profesor</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Usuario_3</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Usuario_4</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Usuario_5</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Usuario_6</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Usuario_7</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Usuario_8</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Usuario_9</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Miguel Centurion</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Usuario_11</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Usuario_12</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Accion</x:t>
+  </x:si>
+  <x:si>
+    <x:t>ISBN</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Titulo</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Prestamo</x:t>
+  </x:si>
+  <x:si>
     <x:t>Libro de Matemáticas</x:t>
   </x:si>
   <x:si>
-    <x:t>Dr. Ana</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Profesor</x:t>
+    <x:t>Miguelon</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Libro 108</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Libro 104</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Devolucion</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Libro 113</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Usuario_10</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Principito</x:t>
+  </x:si>
+  <x:si>
+    <x:t>IdLibro</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Autor</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Disponibilidad</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Autor A</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Disponible</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Libro de Física</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Autor B</x:t>
   </x:si>
   <x:si>
     <x:t>Libro de Historia</x:t>
   </x:si>
   <x:si>
-    <x:t>Usuario_3</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Usuario_4</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Usuario_5</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Usuario_6</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Usuario_7</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Usuario_8</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Usuario_9</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Usuario_10</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Libro de Física</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Usuario_11</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Usuario_12</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Accion</x:t>
-  </x:si>
-  <x:si>
-    <x:t>ISBN</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Titulo</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Prestamo</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Miguelon</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Libro 108</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Libro 104</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Devolucion</x:t>
-  </x:si>
-  <x:si>
-    <x:t>IdLibro</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Autor</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Disponibilidad</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Autor A</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Disponible</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Autor B</x:t>
-  </x:si>
-  <x:si>
     <x:t>Autor C</x:t>
   </x:si>
   <x:si>
@@ -175,9 +181,6 @@
     <x:t>Autor I</x:t>
   </x:si>
   <x:si>
-    <x:t>Libro 113</x:t>
-  </x:si>
-  <x:si>
     <x:t>Autor J</x:t>
   </x:si>
   <x:si>
@@ -185,6 +188,9 @@
   </x:si>
   <x:si>
     <x:t>Libro de Probabilidad</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Antoine de Saint-Exupéry</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -564,7 +570,9 @@
   </x:sheetPr>
   <x:dimension ref="A1:D14"/>
   <x:sheetViews>
-    <x:sheetView workbookViewId="0"/>
+    <x:sheetView tabSelected="1" workbookViewId="0">
+      <x:selection activeCell="M7" sqref="M7"/>
+    </x:sheetView>
   </x:sheetViews>
   <x:sheetFormatPr baseColWidth="10" defaultColWidth="8.853482" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <x:cols>
@@ -584,9 +592,7 @@
       <x:c r="C1" s="1" t="s">
         <x:v>2</x:v>
       </x:c>
-      <x:c r="D1" s="1" t="s">
-        <x:v>3</x:v>
-      </x:c>
+      <x:c r="D1" s="1"/>
     </x:row>
     <x:row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <x:c r="A2" s="0" t="s">
@@ -598,22 +604,16 @@
       <x:c r="C2" s="0" t="s">
         <x:v>2</x:v>
       </x:c>
-      <x:c r="D2" s="0" t="s">
-        <x:v>3</x:v>
-      </x:c>
     </x:row>
     <x:row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <x:c r="A3" s="0">
         <x:v>1</x:v>
       </x:c>
       <x:c r="B3" s="0" t="s">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c r="C3" s="0" t="s">
         <x:v>4</x:v>
-      </x:c>
-      <x:c r="C3" s="0" t="s">
-        <x:v>5</x:v>
-      </x:c>
-      <x:c r="D3" s="0" t="s">
-        <x:v>6</x:v>
       </x:c>
     </x:row>
     <x:row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -621,13 +621,10 @@
         <x:v>2</x:v>
       </x:c>
       <x:c r="B4" s="0" t="s">
-        <x:v>7</x:v>
+        <x:v>5</x:v>
       </x:c>
       <x:c r="C4" s="0" t="s">
-        <x:v>8</x:v>
-      </x:c>
-      <x:c r="D4" s="0" t="s">
-        <x:v>9</x:v>
+        <x:v>6</x:v>
       </x:c>
     </x:row>
     <x:row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -635,13 +632,10 @@
         <x:v>3</x:v>
       </x:c>
       <x:c r="B5" s="0" t="s">
-        <x:v>10</x:v>
+        <x:v>7</x:v>
       </x:c>
       <x:c r="C5" s="0" t="s">
-        <x:v>8</x:v>
-      </x:c>
-      <x:c r="D5" s="0" t="s">
-        <x:v>9</x:v>
+        <x:v>6</x:v>
       </x:c>
     </x:row>
     <x:row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -649,13 +643,10 @@
         <x:v>4</x:v>
       </x:c>
       <x:c r="B6" s="0" t="s">
-        <x:v>11</x:v>
+        <x:v>8</x:v>
       </x:c>
       <x:c r="C6" s="0" t="s">
-        <x:v>8</x:v>
-      </x:c>
-      <x:c r="D6" s="0" t="s">
-        <x:v>9</x:v>
+        <x:v>6</x:v>
       </x:c>
     </x:row>
     <x:row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -663,13 +654,10 @@
         <x:v>5</x:v>
       </x:c>
       <x:c r="B7" s="0" t="s">
-        <x:v>12</x:v>
+        <x:v>9</x:v>
       </x:c>
       <x:c r="C7" s="0" t="s">
-        <x:v>5</x:v>
-      </x:c>
-      <x:c r="D7" s="0" t="s">
-        <x:v>9</x:v>
+        <x:v>4</x:v>
       </x:c>
     </x:row>
     <x:row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -677,13 +665,10 @@
         <x:v>6</x:v>
       </x:c>
       <x:c r="B8" s="0" t="s">
-        <x:v>13</x:v>
+        <x:v>10</x:v>
       </x:c>
       <x:c r="C8" s="0" t="s">
-        <x:v>5</x:v>
-      </x:c>
-      <x:c r="D8" s="0" t="s">
-        <x:v>6</x:v>
+        <x:v>4</x:v>
       </x:c>
     </x:row>
     <x:row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -691,13 +676,10 @@
         <x:v>7</x:v>
       </x:c>
       <x:c r="B9" s="0" t="s">
-        <x:v>14</x:v>
+        <x:v>11</x:v>
       </x:c>
       <x:c r="C9" s="0" t="s">
-        <x:v>5</x:v>
-      </x:c>
-      <x:c r="D9" s="0" t="s">
-        <x:v>6</x:v>
+        <x:v>4</x:v>
       </x:c>
     </x:row>
     <x:row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -705,13 +687,10 @@
         <x:v>8</x:v>
       </x:c>
       <x:c r="B10" s="0" t="s">
-        <x:v>15</x:v>
+        <x:v>12</x:v>
       </x:c>
       <x:c r="C10" s="0" t="s">
-        <x:v>8</x:v>
-      </x:c>
-      <x:c r="D10" s="0" t="s">
-        <x:v>9</x:v>
+        <x:v>6</x:v>
       </x:c>
     </x:row>
     <x:row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -719,12 +698,9 @@
         <x:v>9</x:v>
       </x:c>
       <x:c r="B11" s="0" t="s">
-        <x:v>16</x:v>
+        <x:v>13</x:v>
       </x:c>
       <x:c r="C11" s="0" t="s">
-        <x:v>8</x:v>
-      </x:c>
-      <x:c r="D11" s="0" t="s">
         <x:v>6</x:v>
       </x:c>
     </x:row>
@@ -733,13 +709,10 @@
         <x:v>10</x:v>
       </x:c>
       <x:c r="B12" s="0" t="s">
-        <x:v>17</x:v>
+        <x:v>14</x:v>
       </x:c>
       <x:c r="C12" s="0" t="s">
-        <x:v>5</x:v>
-      </x:c>
-      <x:c r="D12" s="0" t="s">
-        <x:v>18</x:v>
+        <x:v>4</x:v>
       </x:c>
     </x:row>
     <x:row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -747,12 +720,9 @@
         <x:v>11</x:v>
       </x:c>
       <x:c r="B13" s="0" t="s">
-        <x:v>19</x:v>
+        <x:v>15</x:v>
       </x:c>
       <x:c r="C13" s="0" t="s">
-        <x:v>8</x:v>
-      </x:c>
-      <x:c r="D13" s="0" t="s">
         <x:v>6</x:v>
       </x:c>
     </x:row>
@@ -761,13 +731,10 @@
         <x:v>12</x:v>
       </x:c>
       <x:c r="B14" s="0" t="s">
-        <x:v>20</x:v>
+        <x:v>16</x:v>
       </x:c>
       <x:c r="C14" s="0" t="s">
-        <x:v>8</x:v>
-      </x:c>
-      <x:c r="D14" s="0" t="s">
-        <x:v>9</x:v>
+        <x:v>6</x:v>
       </x:c>
     </x:row>
   </x:sheetData>
@@ -784,9 +751,9 @@
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
-  <x:dimension ref="A1:E5"/>
+  <x:dimension ref="A1:E11"/>
   <x:sheetViews>
-    <x:sheetView tabSelected="1" workbookViewId="0">
+    <x:sheetView workbookViewId="0">
       <x:selection activeCell="E4" sqref="E4"/>
     </x:sheetView>
   </x:sheetViews>
@@ -806,13 +773,13 @@
         <x:v>1</x:v>
       </x:c>
       <x:c r="C1" s="1" t="s">
-        <x:v>21</x:v>
+        <x:v>17</x:v>
       </x:c>
       <x:c r="D1" s="1" t="s">
-        <x:v>22</x:v>
+        <x:v>18</x:v>
       </x:c>
       <x:c r="E1" s="1" t="s">
-        <x:v>23</x:v>
+        <x:v>19</x:v>
       </x:c>
     </x:row>
     <x:row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -820,16 +787,16 @@
         <x:v>1</x:v>
       </x:c>
       <x:c r="B2" s="0" t="s">
-        <x:v>4</x:v>
+        <x:v>3</x:v>
       </x:c>
       <x:c r="C2" s="0" t="s">
-        <x:v>24</x:v>
+        <x:v>20</x:v>
       </x:c>
       <x:c r="D2" s="0">
         <x:v>101</x:v>
       </x:c>
       <x:c r="E2" s="0" t="s">
-        <x:v>6</x:v>
+        <x:v>21</x:v>
       </x:c>
     </x:row>
     <x:row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -837,16 +804,16 @@
         <x:v>1</x:v>
       </x:c>
       <x:c r="B3" s="0" t="s">
-        <x:v>4</x:v>
+        <x:v>3</x:v>
       </x:c>
       <x:c r="C3" s="0" t="s">
-        <x:v>24</x:v>
+        <x:v>20</x:v>
       </x:c>
       <x:c r="D3" s="0">
         <x:v>696969</x:v>
       </x:c>
       <x:c r="E3" s="0" t="s">
-        <x:v>25</x:v>
+        <x:v>22</x:v>
       </x:c>
     </x:row>
     <x:row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -854,16 +821,16 @@
         <x:v>1</x:v>
       </x:c>
       <x:c r="B4" s="0" t="s">
-        <x:v>4</x:v>
+        <x:v>3</x:v>
       </x:c>
       <x:c r="C4" s="0" t="s">
-        <x:v>24</x:v>
+        <x:v>20</x:v>
       </x:c>
       <x:c r="D4" s="0">
         <x:v>108</x:v>
       </x:c>
       <x:c r="E4" s="0" t="s">
-        <x:v>26</x:v>
+        <x:v>23</x:v>
       </x:c>
     </x:row>
     <x:row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -871,50 +838,152 @@
         <x:v>1</x:v>
       </x:c>
       <x:c r="B5" s="0" t="s">
-        <x:v>4</x:v>
+        <x:v>3</x:v>
       </x:c>
       <x:c r="C5" s="0" t="s">
-        <x:v>24</x:v>
+        <x:v>20</x:v>
       </x:c>
       <x:c r="D5" s="0">
         <x:v>104</x:v>
       </x:c>
       <x:c r="E5" s="0" t="s">
-        <x:v>27</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="6" spans="1:5">
+        <x:v>24</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <x:c r="A6" s="0">
         <x:v>1</x:v>
       </x:c>
       <x:c r="B6" s="0" t="s">
-        <x:v>4</x:v>
+        <x:v>3</x:v>
       </x:c>
       <x:c r="C6" s="0" t="s">
-        <x:v>28</x:v>
+        <x:v>25</x:v>
       </x:c>
       <x:c r="D6" s="0">
         <x:v>101</x:v>
       </x:c>
       <x:c r="E6" s="0" t="s">
-        <x:v>6</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="7" spans="1:5">
+        <x:v>21</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <x:c r="A7" s="0">
         <x:v>1</x:v>
       </x:c>
       <x:c r="B7" s="0" t="s">
-        <x:v>4</x:v>
+        <x:v>3</x:v>
       </x:c>
       <x:c r="C7" s="0" t="s">
-        <x:v>28</x:v>
+        <x:v>25</x:v>
       </x:c>
       <x:c r="D7" s="0">
         <x:v>696969</x:v>
       </x:c>
       <x:c r="E7" s="0" t="s">
+        <x:v>22</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <x:c r="A8" s="0">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="B8" s="0" t="s">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c r="C8" s="0" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="D8" s="0">
+        <x:v>113</x:v>
+      </x:c>
+      <x:c r="E8" s="0" t="s">
+        <x:v>26</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <x:c r="A9" s="0">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="B9" s="0" t="s">
+        <x:v>27</x:v>
+      </x:c>
+      <x:c r="C9" s="0" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="D9" s="0">
+        <x:v>117</x:v>
+      </x:c>
+      <x:c r="E9" s="0" t="s">
+        <x:v>28</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <x:c r="A10" s="0">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="B10" s="0" t="s">
+        <x:v>27</x:v>
+      </x:c>
+      <x:c r="C10" s="0" t="s">
         <x:v>25</x:v>
+      </x:c>
+      <x:c r="D10" s="0">
+        <x:v>117</x:v>
+      </x:c>
+      <x:c r="E10" s="0" t="s">
+        <x:v>28</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <x:c r="A11" s="0">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="B11" s="0" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="C11" s="0" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="D11" s="0">
+        <x:v>117</x:v>
+      </x:c>
+      <x:c r="E11" s="0" t="s">
+        <x:v>28</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="12" spans="1:5">
+      <x:c r="A12" s="0">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="B12" s="0" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="C12" s="0" t="s">
+        <x:v>25</x:v>
+      </x:c>
+      <x:c r="D12" s="0">
+        <x:v>117</x:v>
+      </x:c>
+      <x:c r="E12" s="0" t="s">
+        <x:v>28</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="13" spans="1:5">
+      <x:c r="A13" s="0">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="B13" s="0" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="C13" s="0" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="D13" s="0">
+        <x:v>117</x:v>
+      </x:c>
+      <x:c r="E13" s="0" t="s">
+        <x:v>28</x:v>
       </x:c>
     </x:row>
   </x:sheetData>
@@ -931,7 +1000,7 @@
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
-  <x:dimension ref="A1:E17"/>
+  <x:dimension ref="A1:E18"/>
   <x:sheetViews>
     <x:sheetView workbookViewId="0">
       <x:selection activeCell="B3" sqref="B3"/>
@@ -949,7 +1018,7 @@
         <x:v>29</x:v>
       </x:c>
       <x:c r="B1" s="1" t="s">
-        <x:v>23</x:v>
+        <x:v>19</x:v>
       </x:c>
       <x:c r="C1" s="1" t="s">
         <x:v>30</x:v>
@@ -964,7 +1033,7 @@
         <x:v>29</x:v>
       </x:c>
       <x:c r="B2" s="0" t="s">
-        <x:v>23</x:v>
+        <x:v>19</x:v>
       </x:c>
       <x:c r="C2" s="0" t="s">
         <x:v>30</x:v>
@@ -978,7 +1047,7 @@
         <x:v>101</x:v>
       </x:c>
       <x:c r="B3" s="0" t="s">
-        <x:v>6</x:v>
+        <x:v>21</x:v>
       </x:c>
       <x:c r="C3" s="0" t="s">
         <x:v>32</x:v>
@@ -992,10 +1061,10 @@
         <x:v>102</x:v>
       </x:c>
       <x:c r="B4" s="0" t="s">
-        <x:v>18</x:v>
+        <x:v>34</x:v>
       </x:c>
       <x:c r="C4" s="0" t="s">
-        <x:v>34</x:v>
+        <x:v>35</x:v>
       </x:c>
       <x:c r="D4" s="0" t="s">
         <x:v>33</x:v>
@@ -1006,13 +1075,13 @@
         <x:v>103</x:v>
       </x:c>
       <x:c r="B5" s="0" t="s">
-        <x:v>9</x:v>
+        <x:v>36</x:v>
       </x:c>
       <x:c r="C5" s="0" t="s">
-        <x:v>35</x:v>
+        <x:v>37</x:v>
       </x:c>
       <x:c r="D5" s="0" t="s">
-        <x:v>36</x:v>
+        <x:v>38</x:v>
       </x:c>
     </x:row>
     <x:row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -1020,13 +1089,13 @@
         <x:v>104</x:v>
       </x:c>
       <x:c r="B6" s="0" t="s">
-        <x:v>27</x:v>
+        <x:v>24</x:v>
       </x:c>
       <x:c r="C6" s="0" t="s">
         <x:v>32</x:v>
       </x:c>
       <x:c r="D6" s="0" t="s">
-        <x:v>36</x:v>
+        <x:v>38</x:v>
       </x:c>
     </x:row>
     <x:row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -1034,10 +1103,10 @@
         <x:v>105</x:v>
       </x:c>
       <x:c r="B7" s="0" t="s">
-        <x:v>37</x:v>
+        <x:v>39</x:v>
       </x:c>
       <x:c r="C7" s="0" t="s">
-        <x:v>34</x:v>
+        <x:v>35</x:v>
       </x:c>
       <x:c r="D7" s="0" t="s">
         <x:v>33</x:v>
@@ -1048,13 +1117,13 @@
         <x:v>106</x:v>
       </x:c>
       <x:c r="B8" s="0" t="s">
+        <x:v>40</x:v>
+      </x:c>
+      <x:c r="C8" s="0" t="s">
+        <x:v>37</x:v>
+      </x:c>
+      <x:c r="D8" s="0" t="s">
         <x:v>38</x:v>
-      </x:c>
-      <x:c r="C8" s="0" t="s">
-        <x:v>35</x:v>
-      </x:c>
-      <x:c r="D8" s="0" t="s">
-        <x:v>36</x:v>
       </x:c>
     </x:row>
     <x:row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -1062,10 +1131,10 @@
         <x:v>107</x:v>
       </x:c>
       <x:c r="B9" s="0" t="s">
-        <x:v>39</x:v>
+        <x:v>41</x:v>
       </x:c>
       <x:c r="C9" s="0" t="s">
-        <x:v>40</x:v>
+        <x:v>42</x:v>
       </x:c>
       <x:c r="D9" s="0" t="s">
         <x:v>33</x:v>
@@ -1076,13 +1145,13 @@
         <x:v>108</x:v>
       </x:c>
       <x:c r="B10" s="0" t="s">
-        <x:v>26</x:v>
+        <x:v>23</x:v>
       </x:c>
       <x:c r="C10" s="0" t="s">
-        <x:v>41</x:v>
+        <x:v>43</x:v>
       </x:c>
       <x:c r="D10" s="0" t="s">
-        <x:v>36</x:v>
+        <x:v>38</x:v>
       </x:c>
     </x:row>
     <x:row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -1090,13 +1159,13 @@
         <x:v>109</x:v>
       </x:c>
       <x:c r="B11" s="0" t="s">
-        <x:v>42</x:v>
+        <x:v>44</x:v>
       </x:c>
       <x:c r="C11" s="0" t="s">
-        <x:v>43</x:v>
+        <x:v>45</x:v>
       </x:c>
       <x:c r="D11" s="0" t="s">
-        <x:v>36</x:v>
+        <x:v>38</x:v>
       </x:c>
     </x:row>
     <x:row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -1104,13 +1173,13 @@
         <x:v>110</x:v>
       </x:c>
       <x:c r="B12" s="0" t="s">
-        <x:v>44</x:v>
+        <x:v>46</x:v>
       </x:c>
       <x:c r="C12" s="0" t="s">
-        <x:v>45</x:v>
+        <x:v>47</x:v>
       </x:c>
       <x:c r="D12" s="0" t="s">
-        <x:v>36</x:v>
+        <x:v>38</x:v>
       </x:c>
     </x:row>
     <x:row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -1118,10 +1187,10 @@
         <x:v>111</x:v>
       </x:c>
       <x:c r="B13" s="0" t="s">
-        <x:v>46</x:v>
+        <x:v>48</x:v>
       </x:c>
       <x:c r="C13" s="0" t="s">
-        <x:v>47</x:v>
+        <x:v>49</x:v>
       </x:c>
       <x:c r="D13" s="0" t="s">
         <x:v>33</x:v>
@@ -1132,13 +1201,13 @@
         <x:v>112</x:v>
       </x:c>
       <x:c r="B14" s="0" t="s">
-        <x:v>48</x:v>
+        <x:v>50</x:v>
       </x:c>
       <x:c r="C14" s="0" t="s">
-        <x:v>49</x:v>
+        <x:v>51</x:v>
       </x:c>
       <x:c r="D14" s="0" t="s">
-        <x:v>36</x:v>
+        <x:v>38</x:v>
       </x:c>
     </x:row>
     <x:row r="15" spans="1:5" x14ac:dyDescent="0.25">
@@ -1146,13 +1215,13 @@
         <x:v>113</x:v>
       </x:c>
       <x:c r="B15" s="0" t="s">
-        <x:v>50</x:v>
+        <x:v>26</x:v>
       </x:c>
       <x:c r="C15" s="0" t="s">
-        <x:v>51</x:v>
+        <x:v>52</x:v>
       </x:c>
       <x:c r="D15" s="0" t="s">
-        <x:v>33</x:v>
+        <x:v>38</x:v>
       </x:c>
     </x:row>
     <x:row r="16" spans="1:5" x14ac:dyDescent="0.25">
@@ -1160,10 +1229,10 @@
         <x:v>696969</x:v>
       </x:c>
       <x:c r="B16" s="0" t="s">
-        <x:v>25</x:v>
+        <x:v>22</x:v>
       </x:c>
       <x:c r="C16" s="0" t="s">
-        <x:v>52</x:v>
+        <x:v>53</x:v>
       </x:c>
       <x:c r="D16" s="0" t="s">
         <x:v>33</x:v>
@@ -1174,13 +1243,27 @@
         <x:v>116</x:v>
       </x:c>
       <x:c r="B17" s="0" t="s">
+        <x:v>54</x:v>
+      </x:c>
+      <x:c r="C17" s="0" t="s">
         <x:v>53</x:v>
-      </x:c>
-      <x:c r="C17" s="0" t="s">
-        <x:v>52</x:v>
       </x:c>
       <x:c r="D17" s="0" t="s">
         <x:v>33</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <x:c r="A18" s="0">
+        <x:v>117</x:v>
+      </x:c>
+      <x:c r="B18" s="0" t="s">
+        <x:v>28</x:v>
+      </x:c>
+      <x:c r="C18" s="0" t="s">
+        <x:v>55</x:v>
+      </x:c>
+      <x:c r="D18" s="0" t="s">
+        <x:v>38</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>

<commit_message>
Separacion en proyectos con independencia de responsabilidades
</commit_message>
<xml_diff>
--- a/CrombieConsole/BibliotecaBaseDatos.xlsx
+++ b/CrombieConsole/BibliotecaBaseDatos.xlsx
@@ -191,6 +191,12 @@
   </x:si>
   <x:si>
     <x:t>Antoine de Saint-Exupéry</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Mi Album de Viaje</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Javier</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -1266,6 +1272,20 @@
         <x:v>38</x:v>
       </x:c>
     </x:row>
+    <x:row r="19" spans="1:5">
+      <x:c r="A19" s="0">
+        <x:v>118</x:v>
+      </x:c>
+      <x:c r="B19" s="0" t="s">
+        <x:v>56</x:v>
+      </x:c>
+      <x:c r="C19" s="0" t="s">
+        <x:v>57</x:v>
+      </x:c>
+      <x:c r="D19" s="0" t="s">
+        <x:v>33</x:v>
+      </x:c>
+    </x:row>
   </x:sheetData>
   <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
   <x:pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Refactorización de servicios y controladores. Añadidos nuevos métodos en LibroController.cs y ProfesorController.cs.
</commit_message>
<xml_diff>
--- a/CrombieConsole/BibliotecaBaseDatos.xlsx
+++ b/CrombieConsole/BibliotecaBaseDatos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\migue\source\repos\Crombie\CrombieConsole\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{109399A2-D635-439E-A853-71DAC24D1E75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DDE3368-24B3-4562-BCDE-71E699E58C13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <x:bookViews>
-    <x:workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="0" activeTab="0" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <x:workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="0" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </x:bookViews>
   <x:sheets>
     <x:sheet name="Usuarios" sheetId="1" r:id="rId1"/>
@@ -112,6 +112,9 @@
     <x:t>Principito</x:t>
   </x:si>
   <x:si>
+    <x:t>Troya</x:t>
+  </x:si>
+  <x:si>
     <x:t>IdLibro</x:t>
   </x:si>
   <x:si>
@@ -197,6 +200,12 @@
   </x:si>
   <x:si>
     <x:t>Javier</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Troya2</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Misterio</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -576,7 +585,7 @@
   </x:sheetPr>
   <x:dimension ref="A1:D14"/>
   <x:sheetViews>
-    <x:sheetView tabSelected="1" workbookViewId="0">
+    <x:sheetView workbookViewId="0">
       <x:selection activeCell="M7" sqref="M7"/>
     </x:sheetView>
   </x:sheetViews>
@@ -757,10 +766,10 @@
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
-  <x:dimension ref="A1:E11"/>
+  <x:dimension ref="A1:E23"/>
   <x:sheetViews>
-    <x:sheetView workbookViewId="0">
-      <x:selection activeCell="E4" sqref="E4"/>
+    <x:sheetView tabSelected="1" workbookViewId="0">
+      <x:selection activeCell="E24" sqref="E24 A24:E24"/>
     </x:sheetView>
   </x:sheetViews>
   <x:sheetFormatPr baseColWidth="10" defaultColWidth="8.853482" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -958,7 +967,7 @@
         <x:v>28</x:v>
       </x:c>
     </x:row>
-    <x:row r="12" spans="1:5">
+    <x:row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <x:c r="A12" s="0">
         <x:v>10</x:v>
       </x:c>
@@ -975,7 +984,7 @@
         <x:v>28</x:v>
       </x:c>
     </x:row>
-    <x:row r="13" spans="1:5">
+    <x:row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <x:c r="A13" s="0">
         <x:v>10</x:v>
       </x:c>
@@ -990,6 +999,210 @@
       </x:c>
       <x:c r="E13" s="0" t="s">
         <x:v>28</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <x:c r="A14" s="0">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="B14" s="0" t="s">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c r="C14" s="0" t="s">
+        <x:v>25</x:v>
+      </x:c>
+      <x:c r="D14" s="0">
+        <x:v>104</x:v>
+      </x:c>
+      <x:c r="E14" s="0" t="s">
+        <x:v>24</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <x:c r="A15" s="0">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="B15" s="0" t="s">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c r="C15" s="0" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="D15" s="0">
+        <x:v>303456</x:v>
+      </x:c>
+      <x:c r="E15" s="0" t="s">
+        <x:v>29</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <x:c r="A16" s="0">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="B16" s="0" t="s">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c r="C16" s="0" t="s">
+        <x:v>25</x:v>
+      </x:c>
+      <x:c r="D16" s="0">
+        <x:v>303456</x:v>
+      </x:c>
+      <x:c r="E16" s="0" t="s">
+        <x:v>29</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <x:c r="A17" s="0">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="B17" s="0" t="s">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c r="C17" s="0" t="s">
+        <x:v>25</x:v>
+      </x:c>
+      <x:c r="D17" s="0">
+        <x:v>113</x:v>
+      </x:c>
+      <x:c r="E17" s="0" t="s">
+        <x:v>26</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <x:c r="A18" s="0">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="B18" s="0" t="s">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c r="C18" s="0" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="D18" s="0">
+        <x:v>303456</x:v>
+      </x:c>
+      <x:c r="E18" s="0" t="s">
+        <x:v>29</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <x:c r="A19" s="0">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="B19" s="0" t="s">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c r="C19" s="0" t="s">
+        <x:v>25</x:v>
+      </x:c>
+      <x:c r="D19" s="0">
+        <x:v>303456</x:v>
+      </x:c>
+      <x:c r="E19" s="0" t="s">
+        <x:v>29</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <x:c r="A20" s="0">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="B20" s="0" t="s">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c r="C20" s="0" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="D20" s="0">
+        <x:v>303456</x:v>
+      </x:c>
+      <x:c r="E20" s="0" t="s">
+        <x:v>29</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <x:c r="A21" s="0">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="B21" s="0" t="s">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c r="C21" s="0" t="s">
+        <x:v>25</x:v>
+      </x:c>
+      <x:c r="D21" s="0">
+        <x:v>303456</x:v>
+      </x:c>
+      <x:c r="E21" s="0" t="s">
+        <x:v>29</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <x:c r="A22" s="0">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="B22" s="0" t="s">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c r="C22" s="0" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="D22" s="0">
+        <x:v>303456</x:v>
+      </x:c>
+      <x:c r="E22" s="0" t="s">
+        <x:v>29</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <x:c r="A23" s="0">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="B23" s="0" t="s">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c r="C23" s="0" t="s">
+        <x:v>25</x:v>
+      </x:c>
+      <x:c r="D23" s="0">
+        <x:v>303456</x:v>
+      </x:c>
+      <x:c r="E23" s="0" t="s">
+        <x:v>29</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="24" spans="1:5">
+      <x:c r="A24" s="0">
+        <x:v>2</x:v>
+      </x:c>
+      <x:c r="B24" s="0" t="s">
+        <x:v>5</x:v>
+      </x:c>
+      <x:c r="C24" s="0" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="D24" s="0">
+        <x:v>101</x:v>
+      </x:c>
+      <x:c r="E24" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="25" spans="1:5">
+      <x:c r="A25" s="0">
+        <x:v>2</x:v>
+      </x:c>
+      <x:c r="B25" s="0" t="s">
+        <x:v>5</x:v>
+      </x:c>
+      <x:c r="C25" s="0" t="s">
+        <x:v>25</x:v>
+      </x:c>
+      <x:c r="D25" s="0">
+        <x:v>101</x:v>
+      </x:c>
+      <x:c r="E25" s="0" t="s">
+        <x:v>21</x:v>
       </x:c>
     </x:row>
   </x:sheetData>
@@ -1006,46 +1219,48 @@
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
-  <x:dimension ref="A1:E18"/>
+  <x:dimension ref="A1:E20"/>
   <x:sheetViews>
     <x:sheetView workbookViewId="0">
-      <x:selection activeCell="B3" sqref="B3"/>
+      <x:selection activeCell="D21" sqref="D21"/>
     </x:sheetView>
   </x:sheetViews>
   <x:sheetFormatPr baseColWidth="10" defaultColWidth="8.853482" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <x:cols>
-    <x:col min="1" max="3" width="8.855469" style="0" customWidth="1"/>
+    <x:col min="1" max="1" width="8.855469" style="0" customWidth="1"/>
+    <x:col min="2" max="2" width="15.855469" style="0" customWidth="1"/>
+    <x:col min="3" max="3" width="19.570312" style="0" customWidth="1"/>
     <x:col min="4" max="4" width="16.710938" style="0" customWidth="1"/>
     <x:col min="5" max="5" width="20.855469" style="0" customWidth="1"/>
   </x:cols>
   <x:sheetData>
     <x:row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <x:c r="A1" s="1" t="s">
-        <x:v>29</x:v>
+        <x:v>30</x:v>
       </x:c>
       <x:c r="B1" s="1" t="s">
         <x:v>19</x:v>
       </x:c>
       <x:c r="C1" s="1" t="s">
-        <x:v>30</x:v>
+        <x:v>31</x:v>
       </x:c>
       <x:c r="D1" s="1" t="s">
-        <x:v>31</x:v>
+        <x:v>32</x:v>
       </x:c>
       <x:c r="E1" s="1"/>
     </x:row>
     <x:row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <x:c r="A2" s="0" t="s">
-        <x:v>29</x:v>
+        <x:v>30</x:v>
       </x:c>
       <x:c r="B2" s="0" t="s">
         <x:v>19</x:v>
       </x:c>
       <x:c r="C2" s="0" t="s">
-        <x:v>30</x:v>
+        <x:v>31</x:v>
       </x:c>
       <x:c r="D2" s="0" t="s">
-        <x:v>31</x:v>
+        <x:v>32</x:v>
       </x:c>
     </x:row>
     <x:row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -1056,10 +1271,10 @@
         <x:v>21</x:v>
       </x:c>
       <x:c r="C3" s="0" t="s">
-        <x:v>32</x:v>
+        <x:v>33</x:v>
       </x:c>
       <x:c r="D3" s="0" t="s">
-        <x:v>33</x:v>
+        <x:v>34</x:v>
       </x:c>
     </x:row>
     <x:row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -1067,13 +1282,13 @@
         <x:v>102</x:v>
       </x:c>
       <x:c r="B4" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="C4" s="0" t="s">
+        <x:v>36</x:v>
+      </x:c>
+      <x:c r="D4" s="0" t="s">
         <x:v>34</x:v>
-      </x:c>
-      <x:c r="C4" s="0" t="s">
-        <x:v>35</x:v>
-      </x:c>
-      <x:c r="D4" s="0" t="s">
-        <x:v>33</x:v>
       </x:c>
     </x:row>
     <x:row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -1081,13 +1296,13 @@
         <x:v>103</x:v>
       </x:c>
       <x:c r="B5" s="0" t="s">
-        <x:v>36</x:v>
+        <x:v>37</x:v>
       </x:c>
       <x:c r="C5" s="0" t="s">
-        <x:v>37</x:v>
+        <x:v>38</x:v>
       </x:c>
       <x:c r="D5" s="0" t="s">
-        <x:v>38</x:v>
+        <x:v>39</x:v>
       </x:c>
     </x:row>
     <x:row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -1098,10 +1313,10 @@
         <x:v>24</x:v>
       </x:c>
       <x:c r="C6" s="0" t="s">
-        <x:v>32</x:v>
+        <x:v>33</x:v>
       </x:c>
       <x:c r="D6" s="0" t="s">
-        <x:v>38</x:v>
+        <x:v>34</x:v>
       </x:c>
     </x:row>
     <x:row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -1109,13 +1324,13 @@
         <x:v>105</x:v>
       </x:c>
       <x:c r="B7" s="0" t="s">
-        <x:v>39</x:v>
+        <x:v>40</x:v>
       </x:c>
       <x:c r="C7" s="0" t="s">
-        <x:v>35</x:v>
+        <x:v>36</x:v>
       </x:c>
       <x:c r="D7" s="0" t="s">
-        <x:v>33</x:v>
+        <x:v>34</x:v>
       </x:c>
     </x:row>
     <x:row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -1123,13 +1338,13 @@
         <x:v>106</x:v>
       </x:c>
       <x:c r="B8" s="0" t="s">
-        <x:v>40</x:v>
+        <x:v>41</x:v>
       </x:c>
       <x:c r="C8" s="0" t="s">
-        <x:v>37</x:v>
+        <x:v>38</x:v>
       </x:c>
       <x:c r="D8" s="0" t="s">
-        <x:v>38</x:v>
+        <x:v>39</x:v>
       </x:c>
     </x:row>
     <x:row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -1137,13 +1352,13 @@
         <x:v>107</x:v>
       </x:c>
       <x:c r="B9" s="0" t="s">
-        <x:v>41</x:v>
+        <x:v>42</x:v>
       </x:c>
       <x:c r="C9" s="0" t="s">
-        <x:v>42</x:v>
+        <x:v>43</x:v>
       </x:c>
       <x:c r="D9" s="0" t="s">
-        <x:v>33</x:v>
+        <x:v>34</x:v>
       </x:c>
     </x:row>
     <x:row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -1154,10 +1369,10 @@
         <x:v>23</x:v>
       </x:c>
       <x:c r="C10" s="0" t="s">
-        <x:v>43</x:v>
+        <x:v>44</x:v>
       </x:c>
       <x:c r="D10" s="0" t="s">
-        <x:v>38</x:v>
+        <x:v>39</x:v>
       </x:c>
     </x:row>
     <x:row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -1165,13 +1380,13 @@
         <x:v>109</x:v>
       </x:c>
       <x:c r="B11" s="0" t="s">
-        <x:v>44</x:v>
+        <x:v>45</x:v>
       </x:c>
       <x:c r="C11" s="0" t="s">
-        <x:v>45</x:v>
+        <x:v>46</x:v>
       </x:c>
       <x:c r="D11" s="0" t="s">
-        <x:v>38</x:v>
+        <x:v>39</x:v>
       </x:c>
     </x:row>
     <x:row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -1179,13 +1394,13 @@
         <x:v>110</x:v>
       </x:c>
       <x:c r="B12" s="0" t="s">
-        <x:v>46</x:v>
+        <x:v>47</x:v>
       </x:c>
       <x:c r="C12" s="0" t="s">
-        <x:v>47</x:v>
+        <x:v>48</x:v>
       </x:c>
       <x:c r="D12" s="0" t="s">
-        <x:v>38</x:v>
+        <x:v>39</x:v>
       </x:c>
     </x:row>
     <x:row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -1193,13 +1408,13 @@
         <x:v>111</x:v>
       </x:c>
       <x:c r="B13" s="0" t="s">
-        <x:v>48</x:v>
+        <x:v>49</x:v>
       </x:c>
       <x:c r="C13" s="0" t="s">
-        <x:v>49</x:v>
+        <x:v>50</x:v>
       </x:c>
       <x:c r="D13" s="0" t="s">
-        <x:v>33</x:v>
+        <x:v>34</x:v>
       </x:c>
     </x:row>
     <x:row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -1207,13 +1422,13 @@
         <x:v>112</x:v>
       </x:c>
       <x:c r="B14" s="0" t="s">
-        <x:v>50</x:v>
+        <x:v>51</x:v>
       </x:c>
       <x:c r="C14" s="0" t="s">
-        <x:v>51</x:v>
+        <x:v>52</x:v>
       </x:c>
       <x:c r="D14" s="0" t="s">
-        <x:v>38</x:v>
+        <x:v>39</x:v>
       </x:c>
     </x:row>
     <x:row r="15" spans="1:5" x14ac:dyDescent="0.25">
@@ -1224,10 +1439,10 @@
         <x:v>26</x:v>
       </x:c>
       <x:c r="C15" s="0" t="s">
-        <x:v>52</x:v>
+        <x:v>53</x:v>
       </x:c>
       <x:c r="D15" s="0" t="s">
-        <x:v>38</x:v>
+        <x:v>34</x:v>
       </x:c>
     </x:row>
     <x:row r="16" spans="1:5" x14ac:dyDescent="0.25">
@@ -1238,10 +1453,10 @@
         <x:v>22</x:v>
       </x:c>
       <x:c r="C16" s="0" t="s">
-        <x:v>53</x:v>
+        <x:v>54</x:v>
       </x:c>
       <x:c r="D16" s="0" t="s">
-        <x:v>33</x:v>
+        <x:v>34</x:v>
       </x:c>
     </x:row>
     <x:row r="17" spans="1:5" x14ac:dyDescent="0.25">
@@ -1249,13 +1464,13 @@
         <x:v>116</x:v>
       </x:c>
       <x:c r="B17" s="0" t="s">
+        <x:v>55</x:v>
+      </x:c>
+      <x:c r="C17" s="0" t="s">
         <x:v>54</x:v>
       </x:c>
-      <x:c r="C17" s="0" t="s">
-        <x:v>53</x:v>
-      </x:c>
       <x:c r="D17" s="0" t="s">
-        <x:v>33</x:v>
+        <x:v>34</x:v>
       </x:c>
     </x:row>
     <x:row r="18" spans="1:5" x14ac:dyDescent="0.25">
@@ -1266,24 +1481,38 @@
         <x:v>28</x:v>
       </x:c>
       <x:c r="C18" s="0" t="s">
-        <x:v>55</x:v>
+        <x:v>56</x:v>
       </x:c>
       <x:c r="D18" s="0" t="s">
-        <x:v>38</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="19" spans="1:5">
+        <x:v>34</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <x:c r="A19" s="0">
         <x:v>118</x:v>
       </x:c>
       <x:c r="B19" s="0" t="s">
-        <x:v>56</x:v>
+        <x:v>57</x:v>
       </x:c>
       <x:c r="C19" s="0" t="s">
-        <x:v>57</x:v>
+        <x:v>58</x:v>
       </x:c>
       <x:c r="D19" s="0" t="s">
-        <x:v>33</x:v>
+        <x:v>34</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <x:c r="A20" s="0">
+        <x:v>303456</x:v>
+      </x:c>
+      <x:c r="B20" s="0" t="s">
+        <x:v>59</x:v>
+      </x:c>
+      <x:c r="C20" s="0" t="s">
+        <x:v>60</x:v>
+      </x:c>
+      <x:c r="D20" s="0" t="s">
+        <x:v>34</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>

<commit_message>
CRUD a traves de Dapper Implementado
</commit_message>
<xml_diff>
--- a/CrombieConsole/BibliotecaBaseDatos.xlsx
+++ b/CrombieConsole/BibliotecaBaseDatos.xlsx
@@ -124,27 +124,27 @@
     <x:t>Disponibilidad</x:t>
   </x:si>
   <x:si>
+    <x:t>Libro de Física</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Autor B</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Disponible</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Libro de Historia</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Autor C</x:t>
+  </x:si>
+  <x:si>
+    <x:t>No Disponible</x:t>
+  </x:si>
+  <x:si>
     <x:t>Autor A</x:t>
   </x:si>
   <x:si>
-    <x:t>Disponible</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Libro de Física</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Autor B</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Libro de Historia</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Autor C</x:t>
-  </x:si>
-  <x:si>
-    <x:t>No Disponible</x:t>
-  </x:si>
-  <x:si>
     <x:t>Libro 105</x:t>
   </x:si>
   <x:si>
@@ -206,6 +206,9 @@
   </x:si>
   <x:si>
     <x:t>Misterio</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Miguel</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -752,6 +755,17 @@
         <x:v>6</x:v>
       </x:c>
     </x:row>
+    <x:row r="15" spans="1:4">
+      <x:c r="A15" s="0">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="B15" s="0" t="s">
+        <x:v>61</x:v>
+      </x:c>
+      <x:c r="C15" s="0" t="s">
+        <x:v>4</x:v>
+      </x:c>
+    </x:row>
   </x:sheetData>
   <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
   <x:pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1268,13 +1282,13 @@
         <x:v>102</x:v>
       </x:c>
       <x:c r="B3" s="0" t="s">
+        <x:v>33</x:v>
+      </x:c>
+      <x:c r="C3" s="0" t="s">
+        <x:v>34</x:v>
+      </x:c>
+      <x:c r="D3" s="0" t="s">
         <x:v>35</x:v>
-      </x:c>
-      <x:c r="C3" s="0" t="s">
-        <x:v>36</x:v>
-      </x:c>
-      <x:c r="D3" s="0" t="s">
-        <x:v>34</x:v>
       </x:c>
     </x:row>
     <x:row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -1282,13 +1296,13 @@
         <x:v>103</x:v>
       </x:c>
       <x:c r="B4" s="0" t="s">
+        <x:v>36</x:v>
+      </x:c>
+      <x:c r="C4" s="0" t="s">
         <x:v>37</x:v>
       </x:c>
-      <x:c r="C4" s="0" t="s">
+      <x:c r="D4" s="0" t="s">
         <x:v>38</x:v>
-      </x:c>
-      <x:c r="D4" s="0" t="s">
-        <x:v>39</x:v>
       </x:c>
     </x:row>
     <x:row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -1299,10 +1313,10 @@
         <x:v>24</x:v>
       </x:c>
       <x:c r="C5" s="0" t="s">
-        <x:v>33</x:v>
+        <x:v>39</x:v>
       </x:c>
       <x:c r="D5" s="0" t="s">
-        <x:v>34</x:v>
+        <x:v>35</x:v>
       </x:c>
     </x:row>
     <x:row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -1313,10 +1327,10 @@
         <x:v>40</x:v>
       </x:c>
       <x:c r="C6" s="0" t="s">
-        <x:v>36</x:v>
+        <x:v>34</x:v>
       </x:c>
       <x:c r="D6" s="0" t="s">
-        <x:v>34</x:v>
+        <x:v>35</x:v>
       </x:c>
     </x:row>
     <x:row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -1327,10 +1341,10 @@
         <x:v>41</x:v>
       </x:c>
       <x:c r="C7" s="0" t="s">
+        <x:v>37</x:v>
+      </x:c>
+      <x:c r="D7" s="0" t="s">
         <x:v>38</x:v>
-      </x:c>
-      <x:c r="D7" s="0" t="s">
-        <x:v>39</x:v>
       </x:c>
     </x:row>
     <x:row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -1344,7 +1358,7 @@
         <x:v>43</x:v>
       </x:c>
       <x:c r="D8" s="0" t="s">
-        <x:v>34</x:v>
+        <x:v>35</x:v>
       </x:c>
     </x:row>
     <x:row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -1358,7 +1372,7 @@
         <x:v>44</x:v>
       </x:c>
       <x:c r="D9" s="0" t="s">
-        <x:v>39</x:v>
+        <x:v>38</x:v>
       </x:c>
     </x:row>
     <x:row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -1372,7 +1386,7 @@
         <x:v>46</x:v>
       </x:c>
       <x:c r="D10" s="0" t="s">
-        <x:v>39</x:v>
+        <x:v>38</x:v>
       </x:c>
     </x:row>
     <x:row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -1386,7 +1400,7 @@
         <x:v>48</x:v>
       </x:c>
       <x:c r="D11" s="0" t="s">
-        <x:v>39</x:v>
+        <x:v>38</x:v>
       </x:c>
     </x:row>
     <x:row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -1400,7 +1414,7 @@
         <x:v>50</x:v>
       </x:c>
       <x:c r="D12" s="0" t="s">
-        <x:v>34</x:v>
+        <x:v>35</x:v>
       </x:c>
     </x:row>
     <x:row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -1414,7 +1428,7 @@
         <x:v>52</x:v>
       </x:c>
       <x:c r="D13" s="0" t="s">
-        <x:v>39</x:v>
+        <x:v>38</x:v>
       </x:c>
     </x:row>
     <x:row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -1428,7 +1442,7 @@
         <x:v>53</x:v>
       </x:c>
       <x:c r="D14" s="0" t="s">
-        <x:v>34</x:v>
+        <x:v>35</x:v>
       </x:c>
     </x:row>
     <x:row r="15" spans="1:5" x14ac:dyDescent="0.25">
@@ -1442,7 +1456,7 @@
         <x:v>54</x:v>
       </x:c>
       <x:c r="D15" s="0" t="s">
-        <x:v>34</x:v>
+        <x:v>35</x:v>
       </x:c>
     </x:row>
     <x:row r="16" spans="1:5" x14ac:dyDescent="0.25">
@@ -1456,7 +1470,7 @@
         <x:v>54</x:v>
       </x:c>
       <x:c r="D16" s="0" t="s">
-        <x:v>34</x:v>
+        <x:v>35</x:v>
       </x:c>
     </x:row>
     <x:row r="17" spans="1:5" x14ac:dyDescent="0.25">
@@ -1470,7 +1484,7 @@
         <x:v>56</x:v>
       </x:c>
       <x:c r="D17" s="0" t="s">
-        <x:v>34</x:v>
+        <x:v>35</x:v>
       </x:c>
     </x:row>
     <x:row r="18" spans="1:5" x14ac:dyDescent="0.25">
@@ -1484,7 +1498,7 @@
         <x:v>58</x:v>
       </x:c>
       <x:c r="D18" s="0" t="s">
-        <x:v>34</x:v>
+        <x:v>35</x:v>
       </x:c>
     </x:row>
     <x:row r="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -1498,7 +1512,7 @@
         <x:v>60</x:v>
       </x:c>
       <x:c r="D19" s="0" t="s">
-        <x:v>34</x:v>
+        <x:v>35</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>